<commit_message>
update new changes on VBA
</commit_message>
<xml_diff>
--- a/ExcelFundamentalsfordataanalysis/week2/week2Practise/122 - Understanding dates.xlsx
+++ b/ExcelFundamentalsfordataanalysis/week2/week2Practise/122 - Understanding dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Data Wrangling MOOC\01 Course 1\02 Week 2\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuliu102\OneDrive - Advanced Micro Devices Inc\Unity_coursera\Excel\ExcelFundamentalsfordataanalysis\week2\week2Practise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073108ED-1A44-41B1-BD2E-33A56F78B32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F68906E-3456-46F7-9241-75E3EA99C98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-4800" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{EC2FC403-3BD3-48C3-93CE-3A4A505B5772}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EC2FC403-3BD3-48C3-93CE-3A4A505B5772}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Invoice Statement" sheetId="2" r:id="rId1"/>
@@ -1247,11 +1247,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1390,32 +1390,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="9"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10"/>
@@ -1423,7 +1423,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1446,16 +1446,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
@@ -1795,31 +1795,31 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="7.453125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="5" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="17" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" style="17" customWidth="1"/>
+    <col min="22" max="22" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>48282.62999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="30">
         <v>24673</v>
       </c>
@@ -1948,7 +1948,7 @@
       <c r="S2" s="34"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="30">
         <v>24673</v>
       </c>
@@ -2010,7 +2010,7 @@
       <c r="R3" s="34"/>
       <c r="S3" s="34"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="30">
         <v>24675</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="R4" s="34"/>
       <c r="S4" s="34"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="30">
         <v>24676</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="R5" s="34"/>
       <c r="S5" s="34"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="30">
         <v>24677</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="R6" s="34"/>
       <c r="S6" s="34"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="30">
         <v>24679</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="30">
         <v>24679</v>
       </c>
@@ -2320,7 +2320,7 @@
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="30">
         <v>24680</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="R9" s="34"/>
       <c r="S9" s="34"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="30">
         <v>24683</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="R10" s="34"/>
       <c r="S10" s="34"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="30">
         <v>24685</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="30">
         <v>24690</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="30">
         <v>24693</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="R13" s="34"/>
       <c r="S13" s="34"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="30">
         <v>24697</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="R14" s="34"/>
       <c r="S14" s="34"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="30">
         <v>24698</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="R15" s="34"/>
       <c r="S15" s="34"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>24699</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="R16" s="34"/>
       <c r="S16" s="34"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="30">
         <v>24704</v>
       </c>
@@ -2878,7 +2878,7 @@
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="30">
         <v>24707</v>
       </c>
@@ -2940,7 +2940,7 @@
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="30">
         <v>24712</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="R19" s="34"/>
       <c r="S19" s="34"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="30">
         <v>24717</v>
       </c>
@@ -3064,7 +3064,7 @@
       <c r="R20" s="34"/>
       <c r="S20" s="34"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="30">
         <v>24722</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="R21" s="34"/>
       <c r="S21" s="34"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="30">
         <v>24727</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="R22" s="34"/>
       <c r="S22" s="34"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="30">
         <v>24730</v>
       </c>
@@ -3250,7 +3250,7 @@
       <c r="R23" s="34"/>
       <c r="S23" s="34"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="30">
         <v>24732</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="R24" s="34"/>
       <c r="S24" s="34"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="30">
         <v>24735</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="R25" s="34"/>
       <c r="S25" s="34"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="30">
         <v>24739</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="R26" s="34"/>
       <c r="S26" s="34"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="30">
         <v>24740</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="R27" s="34"/>
       <c r="S27" s="34"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="30">
         <v>24743</v>
       </c>
@@ -3560,7 +3560,7 @@
       <c r="R28" s="34"/>
       <c r="S28" s="34"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="30">
         <v>24746</v>
       </c>
@@ -3622,7 +3622,7 @@
       <c r="R29" s="34"/>
       <c r="S29" s="34"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="30">
         <v>24750</v>
       </c>
@@ -3684,7 +3684,7 @@
       <c r="R30" s="34"/>
       <c r="S30" s="34"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="30">
         <v>24753</v>
       </c>
@@ -3746,7 +3746,7 @@
       <c r="R31" s="34"/>
       <c r="S31" s="34"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="30">
         <v>24754</v>
       </c>
@@ -3808,7 +3808,7 @@
       <c r="R32" s="34"/>
       <c r="S32" s="34"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="30">
         <v>24756</v>
       </c>
@@ -3870,7 +3870,7 @@
       <c r="R33" s="34"/>
       <c r="S33" s="34"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="30">
         <v>24757</v>
       </c>
@@ -3932,7 +3932,7 @@
       <c r="R34" s="34"/>
       <c r="S34" s="34"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="30">
         <v>24758</v>
       </c>
@@ -3994,7 +3994,7 @@
       <c r="R35" s="34"/>
       <c r="S35" s="34"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>24759</v>
       </c>
@@ -4056,7 +4056,7 @@
       <c r="R36" s="34"/>
       <c r="S36" s="34"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>24760</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="R37" s="34"/>
       <c r="S37" s="34"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>24761</v>
       </c>
@@ -4180,7 +4180,7 @@
       <c r="R38" s="34"/>
       <c r="S38" s="34"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>24764</v>
       </c>
@@ -4242,7 +4242,7 @@
       <c r="R39" s="34"/>
       <c r="S39" s="34"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>24767</v>
       </c>
@@ -4304,7 +4304,7 @@
       <c r="R40" s="34"/>
       <c r="S40" s="34"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>24771</v>
       </c>
@@ -4366,7 +4366,7 @@
       <c r="R41" s="34"/>
       <c r="S41" s="34"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>24775</v>
       </c>
@@ -4428,7 +4428,7 @@
       <c r="R42" s="34"/>
       <c r="S42" s="34"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>24779</v>
       </c>
@@ -4490,7 +4490,7 @@
       <c r="R43" s="34"/>
       <c r="S43" s="34"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>24784</v>
       </c>
@@ -4552,7 +4552,7 @@
       <c r="R44" s="34"/>
       <c r="S44" s="34"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>24788</v>
       </c>
@@ -4614,7 +4614,7 @@
       <c r="R45" s="34"/>
       <c r="S45" s="34"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>24792</v>
       </c>
@@ -4676,7 +4676,7 @@
       <c r="R46" s="34"/>
       <c r="S46" s="34"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>24793</v>
       </c>
@@ -4738,7 +4738,7 @@
       <c r="R47" s="34"/>
       <c r="S47" s="34"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>24795</v>
       </c>
@@ -4800,7 +4800,7 @@
       <c r="R48" s="34"/>
       <c r="S48" s="34"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>24798</v>
       </c>
@@ -4862,7 +4862,7 @@
       <c r="R49" s="34"/>
       <c r="S49" s="34"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>24801</v>
       </c>
@@ -4924,7 +4924,7 @@
       <c r="R50" s="34"/>
       <c r="S50" s="34"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>24803</v>
       </c>
@@ -4986,7 +4986,7 @@
       <c r="R51" s="34"/>
       <c r="S51" s="34"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>24808</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="R52" s="34"/>
       <c r="S52" s="34"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>24813</v>
       </c>
@@ -5110,7 +5110,7 @@
       <c r="R53" s="34"/>
       <c r="S53" s="34"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>24815</v>
       </c>
@@ -5172,7 +5172,7 @@
       <c r="R54" s="34"/>
       <c r="S54" s="34"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>24819</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="R55" s="34"/>
       <c r="S55" s="34"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>24822</v>
       </c>
@@ -5296,7 +5296,7 @@
       <c r="R56" s="34"/>
       <c r="S56" s="34"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>24824</v>
       </c>
@@ -5358,7 +5358,7 @@
       <c r="R57" s="34"/>
       <c r="S57" s="34"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>24825</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="R58" s="34"/>
       <c r="S58" s="34"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>24830</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="R59" s="34"/>
       <c r="S59" s="34"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>24831</v>
       </c>
@@ -5544,7 +5544,7 @@
       <c r="R60" s="34"/>
       <c r="S60" s="34"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>24833</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="R61" s="34"/>
       <c r="S61" s="34"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>24837</v>
       </c>
@@ -5668,7 +5668,7 @@
       <c r="R62" s="34"/>
       <c r="S62" s="34"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>24838</v>
       </c>
@@ -5730,7 +5730,7 @@
       <c r="R63" s="34"/>
       <c r="S63" s="34"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>24842</v>
       </c>
@@ -5792,7 +5792,7 @@
       <c r="R64" s="34"/>
       <c r="S64" s="34"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>24847</v>
       </c>
@@ -5854,7 +5854,7 @@
       <c r="R65" s="34"/>
       <c r="S65" s="34"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>24851</v>
       </c>
@@ -5916,7 +5916,7 @@
       <c r="R66" s="34"/>
       <c r="S66" s="34"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>24854</v>
       </c>
@@ -5978,7 +5978,7 @@
       <c r="R67" s="34"/>
       <c r="S67" s="34"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>24857</v>
       </c>
@@ -6040,7 +6040,7 @@
       <c r="R68" s="34"/>
       <c r="S68" s="34"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>24861</v>
       </c>
@@ -6102,7 +6102,7 @@
       <c r="R69" s="34"/>
       <c r="S69" s="34"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>24863</v>
       </c>
@@ -6164,7 +6164,7 @@
       <c r="R70" s="34"/>
       <c r="S70" s="34"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>24866</v>
       </c>
@@ -6226,7 +6226,7 @@
       <c r="R71" s="34"/>
       <c r="S71" s="34"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>24870</v>
       </c>
@@ -6288,7 +6288,7 @@
       <c r="R72" s="34"/>
       <c r="S72" s="34"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>24873</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="R73" s="34"/>
       <c r="S73" s="34"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>24875</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="R74" s="34"/>
       <c r="S74" s="34"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>24876</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="R75" s="34"/>
       <c r="S75" s="34"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>24877</v>
       </c>
@@ -6536,7 +6536,7 @@
       <c r="R76" s="34"/>
       <c r="S76" s="34"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>24878</v>
       </c>
@@ -6598,7 +6598,7 @@
       <c r="R77" s="34"/>
       <c r="S77" s="34"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>24880</v>
       </c>
@@ -6660,7 +6660,7 @@
       <c r="R78" s="34"/>
       <c r="S78" s="34"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>24882</v>
       </c>
@@ -6722,7 +6722,7 @@
       <c r="R79" s="34"/>
       <c r="S79" s="34"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>24885</v>
       </c>
@@ -6784,7 +6784,7 @@
       <c r="R80" s="34"/>
       <c r="S80" s="34"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>24887</v>
       </c>
@@ -6846,7 +6846,7 @@
       <c r="R81" s="34"/>
       <c r="S81" s="34"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>24891</v>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="R82" s="34"/>
       <c r="S82" s="34"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>24893</v>
       </c>
@@ -6970,7 +6970,7 @@
       <c r="R83" s="34"/>
       <c r="S83" s="34"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>24898</v>
       </c>
@@ -7032,7 +7032,7 @@
       <c r="R84" s="34"/>
       <c r="S84" s="34"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>24902</v>
       </c>
@@ -7097,6 +7097,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0000FF[AMD Official Use Only]&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7105,34 +7108,39 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="5" customWidth="1"/>
+    <col min="9" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" style="5" customWidth="1"/>
     <col min="14" max="14" width="12" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>339</v>
       </c>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="16">
+        <f ca="1">TODAY()</f>
+        <v>44557</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2"/>
       <c r="G2" s="6" t="s">
@@ -7150,12 +7158,12 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>338</v>
       </c>
@@ -7199,7 +7207,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>249</v>
       </c>
@@ -7213,7 +7221,10 @@
       <c r="D5" s="25">
         <v>43892</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25">
+        <f>EDATE(D5,1)</f>
+        <v>43923</v>
+      </c>
       <c r="F5" s="25">
         <v>43938</v>
       </c>
@@ -7233,11 +7244,14 @@
         <f>TEXT(D5,"MMM")</f>
         <v>Mar</v>
       </c>
-      <c r="L5" s="27"/>
+      <c r="L5" s="27">
+        <f>DAY(D5)</f>
+        <v>2</v>
+      </c>
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>249</v>
       </c>
@@ -7250,7 +7264,10 @@
       <c r="D6" s="25">
         <v>43923</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25">
+        <f t="shared" ref="E6:E69" si="0">EDATE(D6,1)</f>
+        <v>43953</v>
+      </c>
       <c r="F6" s="25">
         <v>43941</v>
       </c>
@@ -7267,14 +7284,17 @@
         <v>1021.02</v>
       </c>
       <c r="K6" s="25" t="str">
-        <f t="shared" ref="K6:K69" si="0">TEXT(D6,"MMM")</f>
+        <f t="shared" ref="K6:K69" si="1">TEXT(D6,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="L6" s="27"/>
+      <c r="L6" s="27">
+        <f t="shared" ref="L6:L69" si="2">DAY(D6)</f>
+        <v>2</v>
+      </c>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>254</v>
       </c>
@@ -7287,7 +7307,10 @@
       <c r="D7" s="25">
         <v>43906</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25">
+        <f t="shared" si="0"/>
+        <v>43937</v>
+      </c>
       <c r="F7" s="25">
         <v>43926</v>
       </c>
@@ -7304,14 +7327,17 @@
         <v>409.53</v>
       </c>
       <c r="K7" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L7" s="27"/>
+      <c r="L7" s="27">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>255</v>
       </c>
@@ -7324,7 +7350,10 @@
       <c r="D8" s="25">
         <v>43915</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25">
+        <f t="shared" si="0"/>
+        <v>43946</v>
+      </c>
       <c r="F8" s="25">
         <v>43941</v>
       </c>
@@ -7341,14 +7370,17 @@
         <v>-234.96</v>
       </c>
       <c r="K8" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L8" s="27"/>
+      <c r="L8" s="27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>256</v>
       </c>
@@ -7361,7 +7393,10 @@
       <c r="D9" s="25">
         <v>43907</v>
       </c>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25">
+        <f t="shared" si="0"/>
+        <v>43938</v>
+      </c>
       <c r="F9" s="25">
         <v>43931</v>
       </c>
@@ -7378,14 +7413,17 @@
         <v>-450.12</v>
       </c>
       <c r="K9" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L9" s="27"/>
+      <c r="L9" s="27">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
         <v>257</v>
       </c>
@@ -7398,7 +7436,10 @@
       <c r="D10" s="25">
         <v>43930</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
+        <v>43960</v>
+      </c>
       <c r="F10" s="25">
         <v>43951</v>
       </c>
@@ -7415,14 +7456,17 @@
         <v>114.18</v>
       </c>
       <c r="K10" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L10" s="27"/>
+      <c r="L10" s="27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>258</v>
       </c>
@@ -7435,7 +7479,10 @@
       <c r="D11" s="25">
         <v>43913</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25">
+        <f t="shared" si="0"/>
+        <v>43944</v>
+      </c>
       <c r="F11" s="25">
         <v>43951</v>
       </c>
@@ -7452,14 +7499,17 @@
         <v>930.93</v>
       </c>
       <c r="K11" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L11" s="27"/>
+      <c r="L11" s="27">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>259</v>
       </c>
@@ -7472,7 +7522,10 @@
       <c r="D12" s="25">
         <v>43917</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25">
+        <f t="shared" si="0"/>
+        <v>43948</v>
+      </c>
       <c r="F12" s="25">
         <v>43935</v>
       </c>
@@ -7489,14 +7542,17 @@
         <v>466.29</v>
       </c>
       <c r="K12" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L12" s="27"/>
+      <c r="L12" s="27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>260</v>
       </c>
@@ -7509,7 +7565,10 @@
       <c r="D13" s="25">
         <v>43912</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
       <c r="F13" s="25">
         <v>43948</v>
       </c>
@@ -7526,14 +7585,17 @@
         <v>222.42</v>
       </c>
       <c r="K13" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L13" s="27"/>
+      <c r="L13" s="27">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>261</v>
       </c>
@@ -7546,7 +7608,10 @@
       <c r="D14" s="25">
         <v>43899</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="25">
+        <f t="shared" si="0"/>
+        <v>43930</v>
+      </c>
       <c r="F14" s="25">
         <v>43932</v>
       </c>
@@ -7563,14 +7628,17 @@
         <v>679.8</v>
       </c>
       <c r="K14" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L14" s="27"/>
+      <c r="L14" s="27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>262</v>
       </c>
@@ -7583,7 +7651,10 @@
       <c r="D15" s="25">
         <v>43925</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="25">
+        <f t="shared" si="0"/>
+        <v>43955</v>
+      </c>
       <c r="F15" s="25">
         <v>43944</v>
       </c>
@@ -7600,14 +7671,17 @@
         <v>171.93</v>
       </c>
       <c r="K15" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L15" s="27"/>
+      <c r="L15" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="M15" s="27"/>
       <c r="N15" s="27"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>263</v>
       </c>
@@ -7620,7 +7694,10 @@
       <c r="D16" s="25">
         <v>43885</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="25">
+        <f t="shared" si="0"/>
+        <v>43914</v>
+      </c>
       <c r="F16" s="25">
         <v>43927</v>
       </c>
@@ -7637,14 +7714,17 @@
         <v>623.70000000000005</v>
       </c>
       <c r="K16" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L16" s="27"/>
+      <c r="L16" s="27">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>264</v>
       </c>
@@ -7657,7 +7737,10 @@
       <c r="D17" s="25">
         <v>43919</v>
       </c>
-      <c r="E17" s="25"/>
+      <c r="E17" s="25">
+        <f t="shared" si="0"/>
+        <v>43950</v>
+      </c>
       <c r="F17" s="25">
         <v>43945</v>
       </c>
@@ -7674,14 +7757,17 @@
         <v>221.1</v>
       </c>
       <c r="K17" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L17" s="27"/>
+      <c r="L17" s="27">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
       <c r="M17" s="27"/>
       <c r="N17" s="27"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>265</v>
       </c>
@@ -7694,7 +7780,10 @@
       <c r="D18" s="25">
         <v>43930</v>
       </c>
-      <c r="E18" s="25"/>
+      <c r="E18" s="25">
+        <f t="shared" si="0"/>
+        <v>43960</v>
+      </c>
       <c r="F18" s="25">
         <v>43949</v>
       </c>
@@ -7711,14 +7800,17 @@
         <v>393.36</v>
       </c>
       <c r="K18" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L18" s="27"/>
+      <c r="L18" s="27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
         <v>266</v>
       </c>
@@ -7731,7 +7823,10 @@
       <c r="D19" s="25">
         <v>43899</v>
       </c>
-      <c r="E19" s="25"/>
+      <c r="E19" s="25">
+        <f t="shared" si="0"/>
+        <v>43930</v>
+      </c>
       <c r="F19" s="25">
         <v>43942</v>
       </c>
@@ -7748,14 +7843,17 @@
         <v>642.17999999999995</v>
       </c>
       <c r="K19" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L19" s="27"/>
+      <c r="L19" s="27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="s">
         <v>267</v>
       </c>
@@ -7768,7 +7866,10 @@
       <c r="D20" s="25">
         <v>43909</v>
       </c>
-      <c r="E20" s="25"/>
+      <c r="E20" s="25">
+        <f t="shared" si="0"/>
+        <v>43940</v>
+      </c>
       <c r="F20" s="25">
         <v>43951</v>
       </c>
@@ -7785,14 +7886,17 @@
         <v>499.95</v>
       </c>
       <c r="K20" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L20" s="27"/>
+      <c r="L20" s="27">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
         <v>268</v>
       </c>
@@ -7805,7 +7909,10 @@
       <c r="D21" s="25">
         <v>43890</v>
       </c>
-      <c r="E21" s="25"/>
+      <c r="E21" s="25">
+        <f t="shared" si="0"/>
+        <v>43919</v>
+      </c>
       <c r="F21" s="25">
         <v>43928</v>
       </c>
@@ -7822,14 +7929,17 @@
         <v>299.64</v>
       </c>
       <c r="K21" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L21" s="27"/>
+      <c r="L21" s="27">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>269</v>
       </c>
@@ -7842,7 +7952,10 @@
       <c r="D22" s="25">
         <v>43912</v>
       </c>
-      <c r="E22" s="25"/>
+      <c r="E22" s="25">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
       <c r="F22" s="25">
         <v>43951</v>
       </c>
@@ -7859,14 +7972,17 @@
         <v>312.83999999999997</v>
       </c>
       <c r="K22" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L22" s="27"/>
+      <c r="L22" s="27">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>270</v>
       </c>
@@ -7879,7 +7995,10 @@
       <c r="D23" s="25">
         <v>43904</v>
       </c>
-      <c r="E23" s="25"/>
+      <c r="E23" s="25">
+        <f t="shared" si="0"/>
+        <v>43935</v>
+      </c>
       <c r="F23" s="25">
         <v>43926</v>
       </c>
@@ -7896,14 +8015,17 @@
         <v>993.63</v>
       </c>
       <c r="K23" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L23" s="27"/>
+      <c r="L23" s="27">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
         <v>271</v>
       </c>
@@ -7916,7 +8038,10 @@
       <c r="D24" s="25">
         <v>43917</v>
       </c>
-      <c r="E24" s="25"/>
+      <c r="E24" s="25">
+        <f t="shared" si="0"/>
+        <v>43948</v>
+      </c>
       <c r="F24" s="25">
         <v>43922</v>
       </c>
@@ -7933,14 +8058,17 @@
         <v>1053.69</v>
       </c>
       <c r="K24" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L24" s="27"/>
+      <c r="L24" s="27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>272</v>
       </c>
@@ -7953,7 +8081,10 @@
       <c r="D25" s="25">
         <v>43929</v>
       </c>
-      <c r="E25" s="25"/>
+      <c r="E25" s="25">
+        <f t="shared" si="0"/>
+        <v>43959</v>
+      </c>
       <c r="F25" s="25">
         <v>43951</v>
       </c>
@@ -7970,14 +8101,17 @@
         <v>1047.75</v>
       </c>
       <c r="K25" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L25" s="27"/>
+      <c r="L25" s="27">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>273</v>
       </c>
@@ -7990,7 +8124,10 @@
       <c r="D26" s="25">
         <v>43888</v>
       </c>
-      <c r="E26" s="25"/>
+      <c r="E26" s="25">
+        <f t="shared" si="0"/>
+        <v>43917</v>
+      </c>
       <c r="F26" s="25">
         <v>43929</v>
       </c>
@@ -8007,14 +8144,17 @@
         <v>1096.92</v>
       </c>
       <c r="K26" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L26" s="27"/>
+      <c r="L26" s="27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="24" t="s">
         <v>274</v>
       </c>
@@ -8027,7 +8167,10 @@
       <c r="D27" s="25">
         <v>43886</v>
       </c>
-      <c r="E27" s="25"/>
+      <c r="E27" s="25">
+        <f t="shared" si="0"/>
+        <v>43915</v>
+      </c>
       <c r="F27" s="25">
         <v>43928</v>
       </c>
@@ -8044,14 +8187,17 @@
         <v>257.07</v>
       </c>
       <c r="K27" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L27" s="27"/>
+      <c r="L27" s="27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
         <v>275</v>
       </c>
@@ -8064,7 +8210,10 @@
       <c r="D28" s="25">
         <v>43945</v>
       </c>
-      <c r="E28" s="25"/>
+      <c r="E28" s="25">
+        <f t="shared" si="0"/>
+        <v>43975</v>
+      </c>
       <c r="F28" s="25">
         <v>43949</v>
       </c>
@@ -8081,14 +8230,17 @@
         <v>215.49</v>
       </c>
       <c r="K28" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L28" s="27"/>
+      <c r="L28" s="27">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="24" t="s">
         <v>276</v>
       </c>
@@ -8101,7 +8253,10 @@
       <c r="D29" s="25">
         <v>43926</v>
       </c>
-      <c r="E29" s="25"/>
+      <c r="E29" s="25">
+        <f t="shared" si="0"/>
+        <v>43956</v>
+      </c>
       <c r="F29" s="25">
         <v>43945</v>
       </c>
@@ -8118,14 +8273,17 @@
         <v>455.07</v>
       </c>
       <c r="K29" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L29" s="27"/>
+      <c r="L29" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="24" t="s">
         <v>277</v>
       </c>
@@ -8138,7 +8296,10 @@
       <c r="D30" s="25">
         <v>43923</v>
       </c>
-      <c r="E30" s="25"/>
+      <c r="E30" s="25">
+        <f t="shared" si="0"/>
+        <v>43953</v>
+      </c>
       <c r="F30" s="25">
         <v>43930</v>
       </c>
@@ -8155,14 +8316,17 @@
         <v>711.81</v>
       </c>
       <c r="K30" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L30" s="27"/>
+      <c r="L30" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="24" t="s">
         <v>278</v>
       </c>
@@ -8175,7 +8339,10 @@
       <c r="D31" s="25">
         <v>43911</v>
       </c>
-      <c r="E31" s="25"/>
+      <c r="E31" s="25">
+        <f t="shared" si="0"/>
+        <v>43942</v>
+      </c>
       <c r="F31" s="25">
         <v>43925</v>
       </c>
@@ -8192,14 +8359,17 @@
         <v>78.540000000000006</v>
       </c>
       <c r="K31" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L31" s="27"/>
+      <c r="L31" s="27">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
       <c r="M31" s="27"/>
       <c r="N31" s="27"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="24" t="s">
         <v>279</v>
       </c>
@@ -8212,7 +8382,10 @@
       <c r="D32" s="25">
         <v>43892</v>
       </c>
-      <c r="E32" s="25"/>
+      <c r="E32" s="25">
+        <f t="shared" si="0"/>
+        <v>43923</v>
+      </c>
       <c r="F32" s="25">
         <v>43927</v>
       </c>
@@ -8229,14 +8402,17 @@
         <v>302.61</v>
       </c>
       <c r="K32" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L32" s="27"/>
+      <c r="L32" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="M32" s="27"/>
       <c r="N32" s="27"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="24" t="s">
         <v>280</v>
       </c>
@@ -8249,7 +8425,10 @@
       <c r="D33" s="25">
         <v>43886</v>
       </c>
-      <c r="E33" s="25"/>
+      <c r="E33" s="25">
+        <f t="shared" si="0"/>
+        <v>43915</v>
+      </c>
       <c r="F33" s="25">
         <v>43931</v>
       </c>
@@ -8266,14 +8445,17 @@
         <v>426.03</v>
       </c>
       <c r="K33" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L33" s="27"/>
+      <c r="L33" s="27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="24" t="s">
         <v>281</v>
       </c>
@@ -8286,7 +8468,10 @@
       <c r="D34" s="25">
         <v>43899</v>
       </c>
-      <c r="E34" s="25"/>
+      <c r="E34" s="25">
+        <f t="shared" si="0"/>
+        <v>43930</v>
+      </c>
       <c r="F34" s="25">
         <v>43932</v>
       </c>
@@ -8303,14 +8488,17 @@
         <v>489.72</v>
       </c>
       <c r="K34" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L34" s="27"/>
+      <c r="L34" s="27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="M34" s="27"/>
       <c r="N34" s="27"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="24" t="s">
         <v>282</v>
       </c>
@@ -8323,7 +8511,10 @@
       <c r="D35" s="25">
         <v>43915</v>
       </c>
-      <c r="E35" s="25"/>
+      <c r="E35" s="25">
+        <f t="shared" si="0"/>
+        <v>43946</v>
+      </c>
       <c r="F35" s="25">
         <v>43949</v>
       </c>
@@ -8340,14 +8531,17 @@
         <v>352.44</v>
       </c>
       <c r="K35" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L35" s="27"/>
+      <c r="L35" s="27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="M35" s="27"/>
       <c r="N35" s="27"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="24" t="s">
         <v>283</v>
       </c>
@@ -8360,7 +8554,10 @@
       <c r="D36" s="25">
         <v>43912</v>
       </c>
-      <c r="E36" s="25"/>
+      <c r="E36" s="25">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
       <c r="F36" s="25">
         <v>43937</v>
       </c>
@@ -8377,14 +8574,17 @@
         <v>238.59</v>
       </c>
       <c r="K36" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L36" s="27"/>
+      <c r="L36" s="27">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="24" t="s">
         <v>284</v>
       </c>
@@ -8397,7 +8597,10 @@
       <c r="D37" s="25">
         <v>43936</v>
       </c>
-      <c r="E37" s="25"/>
+      <c r="E37" s="25">
+        <f t="shared" si="0"/>
+        <v>43966</v>
+      </c>
       <c r="F37" s="25">
         <v>43941</v>
       </c>
@@ -8414,14 +8617,17 @@
         <v>549.12</v>
       </c>
       <c r="K37" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L37" s="27"/>
+      <c r="L37" s="27">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
         <v>285</v>
       </c>
@@ -8434,7 +8640,10 @@
       <c r="D38" s="25">
         <v>43893</v>
       </c>
-      <c r="E38" s="25"/>
+      <c r="E38" s="25">
+        <f t="shared" si="0"/>
+        <v>43924</v>
+      </c>
       <c r="F38" s="25">
         <v>43923</v>
       </c>
@@ -8451,14 +8660,17 @@
         <v>322.41000000000003</v>
       </c>
       <c r="K38" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L38" s="27"/>
+      <c r="L38" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>286</v>
       </c>
@@ -8471,7 +8683,10 @@
       <c r="D39" s="25">
         <v>43892</v>
       </c>
-      <c r="E39" s="25"/>
+      <c r="E39" s="25">
+        <f t="shared" si="0"/>
+        <v>43923</v>
+      </c>
       <c r="F39" s="25">
         <v>43934</v>
       </c>
@@ -8488,14 +8703,17 @@
         <v>644.82000000000005</v>
       </c>
       <c r="K39" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L39" s="27"/>
+      <c r="L39" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="24" t="s">
         <v>287</v>
       </c>
@@ -8508,7 +8726,10 @@
       <c r="D40" s="25">
         <v>43923</v>
       </c>
-      <c r="E40" s="25"/>
+      <c r="E40" s="25">
+        <f t="shared" si="0"/>
+        <v>43953</v>
+      </c>
       <c r="F40" s="25">
         <v>43944</v>
       </c>
@@ -8525,14 +8746,17 @@
         <v>113.19</v>
       </c>
       <c r="K40" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L40" s="27"/>
+      <c r="L40" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="24" t="s">
         <v>288</v>
       </c>
@@ -8545,7 +8769,10 @@
       <c r="D41" s="25">
         <v>43941</v>
       </c>
-      <c r="E41" s="25"/>
+      <c r="E41" s="25">
+        <f t="shared" si="0"/>
+        <v>43971</v>
+      </c>
       <c r="F41" s="25">
         <v>43949</v>
       </c>
@@ -8562,14 +8789,17 @@
         <v>449.13</v>
       </c>
       <c r="K41" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L41" s="27"/>
+      <c r="L41" s="27">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
       <c r="M41" s="27"/>
       <c r="N41" s="27"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="24" t="s">
         <v>289</v>
       </c>
@@ -8582,7 +8812,10 @@
       <c r="D42" s="25">
         <v>43911</v>
       </c>
-      <c r="E42" s="25"/>
+      <c r="E42" s="25">
+        <f t="shared" si="0"/>
+        <v>43942</v>
+      </c>
       <c r="F42" s="25">
         <v>43933</v>
       </c>
@@ -8599,14 +8832,17 @@
         <v>819.06</v>
       </c>
       <c r="K42" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L42" s="27"/>
+      <c r="L42" s="27">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
       <c r="M42" s="27"/>
       <c r="N42" s="27"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
         <v>290</v>
       </c>
@@ -8619,7 +8855,10 @@
       <c r="D43" s="25">
         <v>43880</v>
       </c>
-      <c r="E43" s="25"/>
+      <c r="E43" s="25">
+        <f t="shared" si="0"/>
+        <v>43909</v>
+      </c>
       <c r="F43" s="25">
         <v>43924</v>
       </c>
@@ -8636,14 +8875,17 @@
         <v>1019.04</v>
       </c>
       <c r="K43" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L43" s="27"/>
+      <c r="L43" s="27">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
       <c r="M43" s="27"/>
       <c r="N43" s="27"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
         <v>291</v>
       </c>
@@ -8656,7 +8898,10 @@
       <c r="D44" s="25">
         <v>43919</v>
       </c>
-      <c r="E44" s="25"/>
+      <c r="E44" s="25">
+        <f t="shared" si="0"/>
+        <v>43950</v>
+      </c>
       <c r="F44" s="25">
         <v>43935</v>
       </c>
@@ -8673,14 +8918,17 @@
         <v>736.23</v>
       </c>
       <c r="K44" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L44" s="27"/>
+      <c r="L44" s="27">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
       <c r="M44" s="27"/>
       <c r="N44" s="27"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="24" t="s">
         <v>292</v>
       </c>
@@ -8693,7 +8941,10 @@
       <c r="D45" s="25">
         <v>43895</v>
       </c>
-      <c r="E45" s="25"/>
+      <c r="E45" s="25">
+        <f t="shared" si="0"/>
+        <v>43926</v>
+      </c>
       <c r="F45" s="25">
         <v>43937</v>
       </c>
@@ -8710,14 +8961,17 @@
         <v>-600.27</v>
       </c>
       <c r="K45" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L45" s="27"/>
+      <c r="L45" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="M45" s="27"/>
       <c r="N45" s="27"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="24" t="s">
         <v>293</v>
       </c>
@@ -8730,7 +8984,10 @@
       <c r="D46" s="25">
         <v>43907</v>
       </c>
-      <c r="E46" s="25"/>
+      <c r="E46" s="25">
+        <f t="shared" si="0"/>
+        <v>43938</v>
+      </c>
       <c r="F46" s="25">
         <v>43929</v>
       </c>
@@ -8747,14 +9004,17 @@
         <v>480.81</v>
       </c>
       <c r="K46" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L46" s="27"/>
+      <c r="L46" s="27">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="M46" s="27"/>
       <c r="N46" s="27"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
         <v>294</v>
       </c>
@@ -8767,7 +9027,10 @@
       <c r="D47" s="25">
         <v>43908</v>
       </c>
-      <c r="E47" s="25"/>
+      <c r="E47" s="25">
+        <f t="shared" si="0"/>
+        <v>43939</v>
+      </c>
       <c r="F47" s="25">
         <v>43948</v>
       </c>
@@ -8784,14 +9047,17 @@
         <v>253.77</v>
       </c>
       <c r="K47" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L47" s="27"/>
+      <c r="L47" s="27">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="M47" s="27"/>
       <c r="N47" s="27"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="24" t="s">
         <v>295</v>
       </c>
@@ -8804,7 +9070,10 @@
       <c r="D48" s="25">
         <v>43906</v>
       </c>
-      <c r="E48" s="25"/>
+      <c r="E48" s="25">
+        <f t="shared" si="0"/>
+        <v>43937</v>
+      </c>
       <c r="F48" s="25">
         <v>43949</v>
       </c>
@@ -8821,14 +9090,17 @@
         <v>442.86</v>
       </c>
       <c r="K48" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L48" s="27"/>
+      <c r="L48" s="27">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
       <c r="M48" s="27"/>
       <c r="N48" s="27"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
         <v>296</v>
       </c>
@@ -8841,7 +9113,10 @@
       <c r="D49" s="25">
         <v>43901</v>
       </c>
-      <c r="E49" s="25"/>
+      <c r="E49" s="25">
+        <f t="shared" si="0"/>
+        <v>43932</v>
+      </c>
       <c r="F49" s="25">
         <v>43924</v>
       </c>
@@ -8858,14 +9133,17 @@
         <v>630.96</v>
       </c>
       <c r="K49" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L49" s="27"/>
+      <c r="L49" s="27">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
       <c r="M49" s="27"/>
       <c r="N49" s="27"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="24" t="s">
         <v>297</v>
       </c>
@@ -8878,7 +9156,10 @@
       <c r="D50" s="25">
         <v>43895</v>
       </c>
-      <c r="E50" s="25"/>
+      <c r="E50" s="25">
+        <f t="shared" si="0"/>
+        <v>43926</v>
+      </c>
       <c r="F50" s="25">
         <v>43925</v>
       </c>
@@ -8895,14 +9176,17 @@
         <v>821.37</v>
       </c>
       <c r="K50" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L50" s="27"/>
+      <c r="L50" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="M50" s="27"/>
       <c r="N50" s="27"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="24" t="s">
         <v>298</v>
       </c>
@@ -8915,7 +9199,10 @@
       <c r="D51" s="25">
         <v>43888</v>
       </c>
-      <c r="E51" s="25"/>
+      <c r="E51" s="25">
+        <f t="shared" si="0"/>
+        <v>43917</v>
+      </c>
       <c r="F51" s="25">
         <v>43928</v>
       </c>
@@ -8932,14 +9219,17 @@
         <v>950.73</v>
       </c>
       <c r="K51" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L51" s="27"/>
+      <c r="L51" s="27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="M51" s="27"/>
       <c r="N51" s="27"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="24" t="s">
         <v>299</v>
       </c>
@@ -8952,7 +9242,10 @@
       <c r="D52" s="25">
         <v>43921</v>
       </c>
-      <c r="E52" s="25"/>
+      <c r="E52" s="25">
+        <f t="shared" si="0"/>
+        <v>43951</v>
+      </c>
       <c r="F52" s="25">
         <v>43931</v>
       </c>
@@ -8969,14 +9262,17 @@
         <v>956.34</v>
       </c>
       <c r="K52" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L52" s="27"/>
+      <c r="L52" s="27">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
       <c r="M52" s="27"/>
       <c r="N52" s="27"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="24" t="s">
         <v>300</v>
       </c>
@@ -8989,7 +9285,10 @@
       <c r="D53" s="25">
         <v>43917</v>
       </c>
-      <c r="E53" s="25"/>
+      <c r="E53" s="25">
+        <f t="shared" si="0"/>
+        <v>43948</v>
+      </c>
       <c r="F53" s="25">
         <v>43933</v>
       </c>
@@ -9006,14 +9305,17 @@
         <v>1094.28</v>
       </c>
       <c r="K53" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L53" s="27"/>
+      <c r="L53" s="27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="M53" s="27"/>
       <c r="N53" s="27"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="24" t="s">
         <v>301</v>
       </c>
@@ -9026,7 +9328,10 @@
       <c r="D54" s="25">
         <v>43908</v>
       </c>
-      <c r="E54" s="25"/>
+      <c r="E54" s="25">
+        <f t="shared" si="0"/>
+        <v>43939</v>
+      </c>
       <c r="F54" s="25">
         <v>43926</v>
       </c>
@@ -9043,14 +9348,17 @@
         <v>628.98</v>
       </c>
       <c r="K54" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L54" s="27"/>
+      <c r="L54" s="27">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="M54" s="27"/>
       <c r="N54" s="27"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="24" t="s">
         <v>302</v>
       </c>
@@ -9063,7 +9371,10 @@
       <c r="D55" s="25">
         <v>43929</v>
       </c>
-      <c r="E55" s="25"/>
+      <c r="E55" s="25">
+        <f t="shared" si="0"/>
+        <v>43959</v>
+      </c>
       <c r="F55" s="25">
         <v>43941</v>
       </c>
@@ -9080,14 +9391,17 @@
         <v>1058.31</v>
       </c>
       <c r="K55" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L55" s="27"/>
+      <c r="L55" s="27">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="M55" s="27"/>
       <c r="N55" s="27"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="24" t="s">
         <v>303</v>
       </c>
@@ -9100,7 +9414,10 @@
       <c r="D56" s="25">
         <v>43921</v>
       </c>
-      <c r="E56" s="25"/>
+      <c r="E56" s="25">
+        <f t="shared" si="0"/>
+        <v>43951</v>
+      </c>
       <c r="F56" s="25">
         <v>43929</v>
       </c>
@@ -9117,14 +9434,17 @@
         <v>705.54</v>
       </c>
       <c r="K56" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L56" s="27"/>
+      <c r="L56" s="27">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
       <c r="M56" s="27"/>
       <c r="N56" s="27"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="24" t="s">
         <v>304</v>
       </c>
@@ -9137,7 +9457,10 @@
       <c r="D57" s="25">
         <v>43935</v>
       </c>
-      <c r="E57" s="25"/>
+      <c r="E57" s="25">
+        <f t="shared" si="0"/>
+        <v>43965</v>
+      </c>
       <c r="F57" s="25">
         <v>43948</v>
       </c>
@@ -9154,14 +9477,17 @@
         <v>138.6</v>
       </c>
       <c r="K57" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L57" s="27"/>
+      <c r="L57" s="27">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
       <c r="M57" s="27"/>
       <c r="N57" s="27"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="24" t="s">
         <v>305</v>
       </c>
@@ -9174,7 +9500,10 @@
       <c r="D58" s="25">
         <v>43914</v>
       </c>
-      <c r="E58" s="25"/>
+      <c r="E58" s="25">
+        <f t="shared" si="0"/>
+        <v>43945</v>
+      </c>
       <c r="F58" s="25">
         <v>43928</v>
       </c>
@@ -9191,14 +9520,17 @@
         <v>417.12</v>
       </c>
       <c r="K58" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L58" s="27"/>
+      <c r="L58" s="27">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="24" t="s">
         <v>306</v>
       </c>
@@ -9211,7 +9543,10 @@
       <c r="D59" s="25">
         <v>43913</v>
       </c>
-      <c r="E59" s="25"/>
+      <c r="E59" s="25">
+        <f t="shared" si="0"/>
+        <v>43944</v>
+      </c>
       <c r="F59" s="25">
         <v>43939</v>
       </c>
@@ -9228,14 +9563,17 @@
         <v>422.73</v>
       </c>
       <c r="K59" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L59" s="27"/>
+      <c r="L59" s="27">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
       <c r="M59" s="27"/>
       <c r="N59" s="27"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>307</v>
       </c>
@@ -9248,7 +9586,10 @@
       <c r="D60" s="25">
         <v>43908</v>
       </c>
-      <c r="E60" s="25"/>
+      <c r="E60" s="25">
+        <f t="shared" si="0"/>
+        <v>43939</v>
+      </c>
       <c r="F60" s="25">
         <v>43935</v>
       </c>
@@ -9265,14 +9606,17 @@
         <v>1061.94</v>
       </c>
       <c r="K60" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L60" s="27"/>
+      <c r="L60" s="27">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="M60" s="27"/>
       <c r="N60" s="27"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="24" t="s">
         <v>308</v>
       </c>
@@ -9285,7 +9629,10 @@
       <c r="D61" s="25">
         <v>43912</v>
       </c>
-      <c r="E61" s="25"/>
+      <c r="E61" s="25">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
       <c r="F61" s="25">
         <v>43927</v>
       </c>
@@ -9302,14 +9649,17 @@
         <v>602.58000000000004</v>
       </c>
       <c r="K61" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L61" s="27"/>
+      <c r="L61" s="27">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="M61" s="27"/>
       <c r="N61" s="27"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="24" t="s">
         <v>309</v>
       </c>
@@ -9322,7 +9672,10 @@
       <c r="D62" s="25">
         <v>43927</v>
       </c>
-      <c r="E62" s="25"/>
+      <c r="E62" s="25">
+        <f t="shared" si="0"/>
+        <v>43957</v>
+      </c>
       <c r="F62" s="25">
         <v>43951</v>
       </c>
@@ -9339,14 +9692,17 @@
         <v>132.66</v>
       </c>
       <c r="K62" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L62" s="27"/>
+      <c r="L62" s="27">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="M62" s="27"/>
       <c r="N62" s="27"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="24" t="s">
         <v>310</v>
       </c>
@@ -9359,7 +9715,10 @@
       <c r="D63" s="25">
         <v>43896</v>
       </c>
-      <c r="E63" s="25"/>
+      <c r="E63" s="25">
+        <f t="shared" si="0"/>
+        <v>43927</v>
+      </c>
       <c r="F63" s="25">
         <v>43925</v>
       </c>
@@ -9376,14 +9735,17 @@
         <v>56.43</v>
       </c>
       <c r="K63" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L63" s="27"/>
+      <c r="L63" s="27">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="M63" s="27"/>
       <c r="N63" s="27"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="24" t="s">
         <v>311</v>
       </c>
@@ -9396,7 +9758,10 @@
       <c r="D64" s="25">
         <v>43881</v>
       </c>
-      <c r="E64" s="25"/>
+      <c r="E64" s="25">
+        <f t="shared" si="0"/>
+        <v>43910</v>
+      </c>
       <c r="F64" s="25">
         <v>43926</v>
       </c>
@@ -9413,14 +9778,17 @@
         <v>511.83</v>
       </c>
       <c r="K64" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Feb</v>
       </c>
-      <c r="L64" s="27"/>
+      <c r="L64" s="27">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
       <c r="M64" s="27"/>
       <c r="N64" s="27"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="24" t="s">
         <v>312</v>
       </c>
@@ -9433,7 +9801,10 @@
       <c r="D65" s="25">
         <v>43916</v>
       </c>
-      <c r="E65" s="25"/>
+      <c r="E65" s="25">
+        <f t="shared" si="0"/>
+        <v>43947</v>
+      </c>
       <c r="F65" s="25">
         <v>43929</v>
       </c>
@@ -9450,14 +9821,17 @@
         <v>361.02</v>
       </c>
       <c r="K65" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L65" s="27"/>
+      <c r="L65" s="27">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
       <c r="M65" s="27"/>
       <c r="N65" s="27"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="24" t="s">
         <v>313</v>
       </c>
@@ -9470,7 +9844,10 @@
       <c r="D66" s="25">
         <v>43932</v>
       </c>
-      <c r="E66" s="25"/>
+      <c r="E66" s="25">
+        <f t="shared" si="0"/>
+        <v>43962</v>
+      </c>
       <c r="F66" s="25">
         <v>43948</v>
       </c>
@@ -9487,14 +9864,17 @@
         <v>668.25</v>
       </c>
       <c r="K66" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L66" s="27"/>
+      <c r="L66" s="27">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
       <c r="M66" s="27"/>
       <c r="N66" s="27"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="24" t="s">
         <v>314</v>
       </c>
@@ -9507,7 +9887,10 @@
       <c r="D67" s="25">
         <v>43914</v>
       </c>
-      <c r="E67" s="25"/>
+      <c r="E67" s="25">
+        <f t="shared" si="0"/>
+        <v>43945</v>
+      </c>
       <c r="F67" s="25">
         <v>43933</v>
       </c>
@@ -9524,14 +9907,17 @@
         <v>126.72</v>
       </c>
       <c r="K67" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L67" s="27"/>
+      <c r="L67" s="27">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="M67" s="27"/>
       <c r="N67" s="27"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="24" t="s">
         <v>315</v>
       </c>
@@ -9544,7 +9930,10 @@
       <c r="D68" s="25">
         <v>43905</v>
       </c>
-      <c r="E68" s="25"/>
+      <c r="E68" s="25">
+        <f t="shared" si="0"/>
+        <v>43936</v>
+      </c>
       <c r="F68" s="25">
         <v>43943</v>
       </c>
@@ -9561,14 +9950,17 @@
         <v>1000.23</v>
       </c>
       <c r="K68" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L68" s="27"/>
+      <c r="L68" s="27">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="M68" s="27"/>
       <c r="N68" s="27"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="24" t="s">
         <v>316</v>
       </c>
@@ -9581,7 +9973,10 @@
       <c r="D69" s="25">
         <v>43918</v>
       </c>
-      <c r="E69" s="25"/>
+      <c r="E69" s="25">
+        <f t="shared" si="0"/>
+        <v>43949</v>
+      </c>
       <c r="F69" s="25">
         <v>43939</v>
       </c>
@@ -9598,14 +9993,17 @@
         <v>948.75</v>
       </c>
       <c r="K69" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L69" s="27"/>
+      <c r="L69" s="27">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
       <c r="M69" s="27"/>
       <c r="N69" s="27"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="24" t="s">
         <v>317</v>
       </c>
@@ -9618,7 +10016,10 @@
       <c r="D70" s="25">
         <v>43904</v>
       </c>
-      <c r="E70" s="25"/>
+      <c r="E70" s="25">
+        <f t="shared" ref="E70:E88" si="3">EDATE(D70,1)</f>
+        <v>43935</v>
+      </c>
       <c r="F70" s="25">
         <v>43937</v>
       </c>
@@ -9635,14 +10036,17 @@
         <v>446.49</v>
       </c>
       <c r="K70" s="25" t="str">
-        <f t="shared" ref="K70:K88" si="1">TEXT(D70,"MMM")</f>
+        <f t="shared" ref="K70:K88" si="4">TEXT(D70,"MMM")</f>
         <v>Mar</v>
       </c>
-      <c r="L70" s="27"/>
+      <c r="L70" s="27">
+        <f t="shared" ref="L70:L88" si="5">DAY(D70)</f>
+        <v>14</v>
+      </c>
       <c r="M70" s="27"/>
       <c r="N70" s="27"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="24" t="s">
         <v>318</v>
       </c>
@@ -9655,7 +10059,10 @@
       <c r="D71" s="25">
         <v>43933</v>
       </c>
-      <c r="E71" s="25"/>
+      <c r="E71" s="25">
+        <f t="shared" si="3"/>
+        <v>43963</v>
+      </c>
       <c r="F71" s="25">
         <v>43940</v>
       </c>
@@ -9672,14 +10079,17 @@
         <v>242.22</v>
       </c>
       <c r="K71" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Apr</v>
       </c>
-      <c r="L71" s="27"/>
+      <c r="L71" s="27">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
       <c r="M71" s="27"/>
       <c r="N71" s="27"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="24" t="s">
         <v>319</v>
       </c>
@@ -9692,7 +10102,10 @@
       <c r="D72" s="25">
         <v>43887</v>
       </c>
-      <c r="E72" s="25"/>
+      <c r="E72" s="25">
+        <f t="shared" si="3"/>
+        <v>43916</v>
+      </c>
       <c r="F72" s="25">
         <v>43929</v>
       </c>
@@ -9709,14 +10122,17 @@
         <v>600.6</v>
       </c>
       <c r="K72" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Feb</v>
       </c>
-      <c r="L72" s="27"/>
+      <c r="L72" s="27">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
       <c r="M72" s="27"/>
       <c r="N72" s="27"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="24" t="s">
         <v>320</v>
       </c>
@@ -9729,7 +10145,10 @@
       <c r="D73" s="25">
         <v>43905</v>
       </c>
-      <c r="E73" s="25"/>
+      <c r="E73" s="25">
+        <f t="shared" si="3"/>
+        <v>43936</v>
+      </c>
       <c r="F73" s="25">
         <v>43942</v>
       </c>
@@ -9746,14 +10165,17 @@
         <v>546.80999999999995</v>
       </c>
       <c r="K73" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L73" s="27"/>
+      <c r="L73" s="27">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
       <c r="M73" s="27"/>
       <c r="N73" s="27"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="24" t="s">
         <v>321</v>
       </c>
@@ -9766,7 +10188,10 @@
       <c r="D74" s="25">
         <v>43900</v>
       </c>
-      <c r="E74" s="25"/>
+      <c r="E74" s="25">
+        <f t="shared" si="3"/>
+        <v>43931</v>
+      </c>
       <c r="F74" s="25">
         <v>43931</v>
       </c>
@@ -9783,14 +10208,17 @@
         <v>840.51</v>
       </c>
       <c r="K74" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L74" s="27"/>
+      <c r="L74" s="27">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="M74" s="27"/>
       <c r="N74" s="27"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="24" t="s">
         <v>322</v>
       </c>
@@ -9803,7 +10231,10 @@
       <c r="D75" s="25">
         <v>43923</v>
       </c>
-      <c r="E75" s="25"/>
+      <c r="E75" s="25">
+        <f t="shared" si="3"/>
+        <v>43953</v>
+      </c>
       <c r="F75" s="25">
         <v>43951</v>
       </c>
@@ -9820,14 +10251,17 @@
         <v>603.57000000000005</v>
       </c>
       <c r="K75" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Apr</v>
       </c>
-      <c r="L75" s="27"/>
+      <c r="L75" s="27">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="M75" s="27"/>
       <c r="N75" s="27"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="24" t="s">
         <v>323</v>
       </c>
@@ -9840,7 +10274,10 @@
       <c r="D76" s="25">
         <v>43914</v>
       </c>
-      <c r="E76" s="25"/>
+      <c r="E76" s="25">
+        <f t="shared" si="3"/>
+        <v>43945</v>
+      </c>
       <c r="F76" s="25">
         <v>43944</v>
       </c>
@@ -9857,14 +10294,17 @@
         <v>816.75</v>
       </c>
       <c r="K76" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L76" s="27"/>
+      <c r="L76" s="27">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
       <c r="M76" s="27"/>
       <c r="N76" s="27"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="24" t="s">
         <v>324</v>
       </c>
@@ -9877,7 +10317,10 @@
       <c r="D77" s="25">
         <v>43912</v>
       </c>
-      <c r="E77" s="25"/>
+      <c r="E77" s="25">
+        <f t="shared" si="3"/>
+        <v>43943</v>
+      </c>
       <c r="F77" s="25">
         <v>43951</v>
       </c>
@@ -9894,14 +10337,17 @@
         <v>1065.57</v>
       </c>
       <c r="K77" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L77" s="27"/>
+      <c r="L77" s="27">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
       <c r="M77" s="27"/>
       <c r="N77" s="27"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="24" t="s">
         <v>325</v>
       </c>
@@ -9914,7 +10360,10 @@
       <c r="D78" s="25">
         <v>43919</v>
       </c>
-      <c r="E78" s="25"/>
+      <c r="E78" s="25">
+        <f t="shared" si="3"/>
+        <v>43950</v>
+      </c>
       <c r="F78" s="25">
         <v>43925</v>
       </c>
@@ -9931,14 +10380,17 @@
         <v>523.38</v>
       </c>
       <c r="K78" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L78" s="27"/>
+      <c r="L78" s="27">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
       <c r="M78" s="27"/>
       <c r="N78" s="27"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="24" t="s">
         <v>326</v>
       </c>
@@ -9951,7 +10403,10 @@
       <c r="D79" s="25">
         <v>43890</v>
       </c>
-      <c r="E79" s="25"/>
+      <c r="E79" s="25">
+        <f t="shared" si="3"/>
+        <v>43919</v>
+      </c>
       <c r="F79" s="25">
         <v>43932</v>
       </c>
@@ -9968,14 +10423,17 @@
         <v>650.42999999999995</v>
       </c>
       <c r="K79" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Feb</v>
       </c>
-      <c r="L79" s="27"/>
+      <c r="L79" s="27">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
       <c r="M79" s="27"/>
       <c r="N79" s="27"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="24" t="s">
         <v>327</v>
       </c>
@@ -9988,7 +10446,10 @@
       <c r="D80" s="25">
         <v>43934</v>
       </c>
-      <c r="E80" s="25"/>
+      <c r="E80" s="25">
+        <f t="shared" si="3"/>
+        <v>43964</v>
+      </c>
       <c r="F80" s="25">
         <v>43943</v>
       </c>
@@ -10005,14 +10466,17 @@
         <v>809.49</v>
       </c>
       <c r="K80" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Apr</v>
       </c>
-      <c r="L80" s="27"/>
+      <c r="L80" s="27">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
       <c r="M80" s="27"/>
       <c r="N80" s="27"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="24" t="s">
         <v>328</v>
       </c>
@@ -10025,7 +10489,10 @@
       <c r="D81" s="25">
         <v>43901</v>
       </c>
-      <c r="E81" s="25"/>
+      <c r="E81" s="25">
+        <f t="shared" si="3"/>
+        <v>43932</v>
+      </c>
       <c r="F81" s="25">
         <v>43943</v>
       </c>
@@ -10042,14 +10509,17 @@
         <v>424.38</v>
       </c>
       <c r="K81" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L81" s="27"/>
+      <c r="L81" s="27">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
       <c r="M81" s="27"/>
       <c r="N81" s="27"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="24" t="s">
         <v>329</v>
       </c>
@@ -10062,7 +10532,10 @@
       <c r="D82" s="25">
         <v>43933</v>
       </c>
-      <c r="E82" s="25"/>
+      <c r="E82" s="25">
+        <f t="shared" si="3"/>
+        <v>43963</v>
+      </c>
       <c r="F82" s="25">
         <v>43935</v>
       </c>
@@ -10079,14 +10552,17 @@
         <v>955.68</v>
       </c>
       <c r="K82" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Apr</v>
       </c>
-      <c r="L82" s="27"/>
+      <c r="L82" s="27">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
       <c r="M82" s="27"/>
       <c r="N82" s="27"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="24" t="s">
         <v>330</v>
       </c>
@@ -10099,7 +10575,10 @@
       <c r="D83" s="25">
         <v>43942</v>
       </c>
-      <c r="E83" s="25"/>
+      <c r="E83" s="25">
+        <f t="shared" si="3"/>
+        <v>43972</v>
+      </c>
       <c r="F83" s="25">
         <v>43950</v>
       </c>
@@ -10116,14 +10595,17 @@
         <v>764.28</v>
       </c>
       <c r="K83" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Apr</v>
       </c>
-      <c r="L83" s="27"/>
+      <c r="L83" s="27">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
       <c r="M83" s="27"/>
       <c r="N83" s="27"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="24" t="s">
         <v>331</v>
       </c>
@@ -10136,7 +10618,10 @@
       <c r="D84" s="25">
         <v>43897</v>
       </c>
-      <c r="E84" s="25"/>
+      <c r="E84" s="25">
+        <f t="shared" si="3"/>
+        <v>43928</v>
+      </c>
       <c r="F84" s="25">
         <v>43926</v>
       </c>
@@ -10153,14 +10638,17 @@
         <v>335.61</v>
       </c>
       <c r="K84" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L84" s="27"/>
+      <c r="L84" s="27">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="M84" s="27"/>
       <c r="N84" s="27"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="24" t="s">
         <v>332</v>
       </c>
@@ -10173,7 +10661,10 @@
       <c r="D85" s="25">
         <v>43898</v>
       </c>
-      <c r="E85" s="25"/>
+      <c r="E85" s="25">
+        <f t="shared" si="3"/>
+        <v>43929</v>
+      </c>
       <c r="F85" s="25">
         <v>43940</v>
       </c>
@@ -10190,14 +10681,17 @@
         <v>763.29</v>
       </c>
       <c r="K85" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L85" s="27"/>
+      <c r="L85" s="27">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="M85" s="27"/>
       <c r="N85" s="27"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
         <v>333</v>
       </c>
@@ -10210,7 +10704,10 @@
       <c r="D86" s="25">
         <v>43919</v>
       </c>
-      <c r="E86" s="25"/>
+      <c r="E86" s="25">
+        <f t="shared" si="3"/>
+        <v>43950</v>
+      </c>
       <c r="F86" s="25">
         <v>43933</v>
       </c>
@@ -10227,14 +10724,17 @@
         <v>446.16</v>
       </c>
       <c r="K86" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L86" s="27"/>
+      <c r="L86" s="27">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
       <c r="M86" s="27"/>
       <c r="N86" s="27"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="24" t="s">
         <v>334</v>
       </c>
@@ -10247,7 +10747,10 @@
       <c r="D87" s="25">
         <v>43898</v>
       </c>
-      <c r="E87" s="25"/>
+      <c r="E87" s="25">
+        <f t="shared" si="3"/>
+        <v>43929</v>
+      </c>
       <c r="F87" s="25">
         <v>43941</v>
       </c>
@@ -10264,14 +10767,17 @@
         <v>1032.24</v>
       </c>
       <c r="K87" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L87" s="27"/>
+      <c r="L87" s="27">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="M87" s="27"/>
       <c r="N87" s="27"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="24" t="s">
         <v>335</v>
       </c>
@@ -10284,7 +10790,10 @@
       <c r="D88" s="25">
         <v>43915</v>
       </c>
-      <c r="E88" s="25"/>
+      <c r="E88" s="25">
+        <f t="shared" si="3"/>
+        <v>43946</v>
+      </c>
       <c r="F88" s="25">
         <v>43933</v>
       </c>
@@ -10301,10 +10810,13 @@
         <v>533.28</v>
       </c>
       <c r="K88" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>Mar</v>
       </c>
-      <c r="L88" s="27"/>
+      <c r="L88" s="27">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
       <c r="M88" s="27"/>
       <c r="N88" s="27"/>
     </row>
@@ -10320,6 +10832,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0000FF[AMD Official Use Only]&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -10331,13 +10846,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="4" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>346</v>
       </c>
@@ -10345,26 +10860,26 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>348</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>347</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>349</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>350</v>
       </c>
@@ -10378,23 +10893,27 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>251</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>253</v>
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0000FF[AMD Official Use Only]&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -10404,22 +10923,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="16" customWidth="1"/>
     <col min="2" max="2" width="9" style="4"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="21" t="s">
         <v>380</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>365</v>
       </c>
@@ -10430,7 +10949,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>43831</v>
       </c>
@@ -10442,7 +10961,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>43857</v>
       </c>
@@ -10454,7 +10973,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>43931</v>
       </c>
@@ -10466,7 +10985,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>43932</v>
       </c>
@@ -10478,7 +10997,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>43933</v>
       </c>
@@ -10490,7 +11009,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>43934</v>
       </c>
@@ -10502,7 +11021,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>43946</v>
       </c>
@@ -10514,7 +11033,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>43990</v>
       </c>
@@ -10526,7 +11045,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>44109</v>
       </c>
@@ -10538,7 +11057,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>44190</v>
       </c>
@@ -10550,7 +11069,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>44191</v>
       </c>
@@ -10562,7 +11081,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="16">
         <v>44193</v>
       </c>
@@ -10574,13 +11093,13 @@
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>396</v>
       </c>
       <c r="B19"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>397</v>
       </c>
@@ -10589,7 +11108,7 @@
       </c>
       <c r="C20" s="20"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>381</v>
       </c>
@@ -10597,7 +11116,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -10605,7 +11124,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -10613,7 +11132,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4</v>
       </c>
@@ -10621,7 +11140,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
@@ -10629,7 +11148,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>6</v>
       </c>
@@ -10637,7 +11156,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>7</v>
       </c>
@@ -10645,7 +11164,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11</v>
       </c>
@@ -10653,7 +11172,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12</v>
       </c>
@@ -10661,7 +11180,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>13</v>
       </c>
@@ -10669,7 +11188,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14</v>
       </c>
@@ -10677,7 +11196,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -10685,7 +11204,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
@@ -10693,7 +11212,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
@@ -10701,7 +11220,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>399</v>
       </c>
@@ -10709,5 +11228,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0000FF[AMD Official Use Only]&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>